<commit_message>
updated documentation and TOE chart
</commit_message>
<xml_diff>
--- a/toeChart_finalProject.xlsx
+++ b/toeChart_finalProject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PCC\CIS 036\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PCC\CIS 036\cis036_finalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934451C2-B14C-4E99-99EE-40F80A53C92B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE764F63-9A0D-4B99-AA9C-235F186E2AB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21624" windowHeight="9648" xr2:uid="{B5D8C502-03EB-4DDC-8909-F79038F382E6}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -57,6 +57,66 @@
   </si>
   <si>
     <t>Insert values into User table</t>
+  </si>
+  <si>
+    <t>btnLogin</t>
+  </si>
+  <si>
+    <t>Checks if username and password matches Fit_User table</t>
+  </si>
+  <si>
+    <t>btnCancel</t>
+  </si>
+  <si>
+    <t>Exit program</t>
+  </si>
+  <si>
+    <t>txtUsername, txtPassword</t>
+  </si>
+  <si>
+    <t>Login values</t>
+  </si>
+  <si>
+    <t>btnRegister</t>
+  </si>
+  <si>
+    <t>Open registration form, hide login form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lblName, lblDateDisplay, lblAgeDisplay, </t>
+  </si>
+  <si>
+    <t>Displays user name, today's date and age for profile info</t>
+  </si>
+  <si>
+    <t>lblInitWt, lblCurrBMI, lblNewBMI</t>
+  </si>
+  <si>
+    <t>Displays initial weight given at registration, current BMI based on initial weight and new BMI based on new weight</t>
+  </si>
+  <si>
+    <t>btnCalcBMI</t>
+  </si>
+  <si>
+    <t>Calculates BMI based on new weight entered</t>
+  </si>
+  <si>
+    <t>txtNewWt</t>
+  </si>
+  <si>
+    <t>New weight value entered</t>
+  </si>
+  <si>
+    <t>txtAbdominal, txtNeck, txtHips</t>
+  </si>
+  <si>
+    <t>Values for calculating body fat based on circumference</t>
+  </si>
+  <si>
+    <t>btnCalcBF</t>
+  </si>
+  <si>
+    <t>Calculates body fat based on circumference values</t>
   </si>
 </sst>
 </file>
@@ -80,15 +140,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,20 +174,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,49 +533,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409C2C6-233A-4628-91D7-9F93CBCC88AC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="33.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="33.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add pseudocode + flwochart
</commit_message>
<xml_diff>
--- a/toeChart_finalProject.xlsx
+++ b/toeChart_finalProject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PCC\CIS 036\cis036_finalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE764F63-9A0D-4B99-AA9C-235F186E2AB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C1D5B6-DD55-4C0B-A3CB-2CD036CB04AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21624" windowHeight="9648" xr2:uid="{B5D8C502-03EB-4DDC-8909-F79038F382E6}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Task</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Checks if username and password matches Fit_User table</t>
   </si>
   <si>
-    <t>btnCancel</t>
-  </si>
-  <si>
     <t>Exit program</t>
   </si>
   <si>
@@ -117,6 +114,15 @@
   </si>
   <si>
     <t>Calculates body fat based on circumference values</t>
+  </si>
+  <si>
+    <t>frmLogin.btnCancel</t>
+  </si>
+  <si>
+    <t>Return to login</t>
+  </si>
+  <si>
+    <t>frmUserInfo.btnCancel</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A409C2C6-233A-4628-91D7-9F93CBCC88AC}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,10 +574,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>5</v>
@@ -579,10 +585,10 @@
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>5</v>
@@ -590,10 +596,10 @@
     </row>
     <row r="5" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -601,10 +607,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -612,10 +618,10 @@
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
@@ -645,32 +651,32 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>4</v>
@@ -678,12 +684,23 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>